<commit_message>
Updates task import template
</commit_message>
<xml_diff>
--- a/information/taskImportTemplate.xlsx
+++ b/information/taskImportTemplate.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mae002\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elias/Documents/PsyTestPro/information/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC3B13C-BF8F-8349-8DD8-FEEBFA12D457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="765" windowWidth="28035" windowHeight="17280"/>
+    <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tasks" sheetId="1" r:id="rId1"/>
@@ -19,17 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -70,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -105,7 +95,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -130,10 +120,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -149,7 +139,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6756400" y="406400"/>
-          <a:ext cx="3911600" cy="2679700"/>
+          <a:ext cx="4470400" cy="4191000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -235,6 +225,141 @@
             <a:rPr lang="en-US" sz="1200" baseline="0"/>
             <a:t>Description (Optional to title): Description</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0"/>
+            <a:t>Variables:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>{id} -&gt; Participant ID</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>{experiment} -&gt; Experiment Name</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>{startTime} -&gt; Time when the experiment started</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>{timestamp} -&gt; Current time stamp. Format: YYYY.mm.dd hh:mm:ss</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>{scriptCount} -&gt; A counter that increments with each execution of the command within a task (used conly for commands)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="0"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -539,20 +664,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -569,7 +694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -580,7 +705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -594,109 +719,109 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Task now have a duration - from now on the task has a duration instead of a start time. so the user only has to define how long a task takes. the next tasks starts when this task ends.
</commit_message>
<xml_diff>
--- a/information/taskImportTemplate.xlsx
+++ b/information/taskImportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elias/Documents/PsyTestPro/information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC3B13C-BF8F-8349-8DD8-FEEBFA12D457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38718A1-06B5-194E-96E8-F29B31861BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>minutes</t>
-  </si>
-  <si>
     <t>py ./scripts/myScript.py</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>welcome</t>
+  </si>
+  <si>
+    <t>duration in minutes</t>
   </si>
 </sst>
 </file>
@@ -190,7 +190,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" baseline="0"/>
-            <a:t> The name of the task.</a:t>
+            <a:t> The name of the task. Must be unique</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -199,7 +199,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" baseline="0"/>
-            <a:t>minutes. When the task will start after the last task (First task: Minutes after the experiment was started)</a:t>
+            <a:t>minutes. How long the task takes.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -668,7 +668,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -682,7 +682,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -696,27 +696,27 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>10</v>
       </c>
       <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Adds tasks which open urls instead of text screen or command
</commit_message>
<xml_diff>
--- a/information/taskImportTemplate.xlsx
+++ b/information/taskImportTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elias/Documents/PsyTestPro/information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A477296F-C379-7849-A3CB-7DFA6DD91589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626D4864-46C4-624D-AA5B-C2CF26EB200F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>task_name</t>
   </si>
@@ -55,16 +55,30 @@
   </si>
   <si>
     <t>duration in minutes</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>https://www.google.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -87,14 +101,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -115,15 +132,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -138,8 +155,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6756400" y="406400"/>
-          <a:ext cx="4470400" cy="4191000"/>
+          <a:off x="7213600" y="419100"/>
+          <a:ext cx="4470400" cy="4699000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -224,6 +241,21 @@
           <a:r>
             <a:rPr lang="en-US" sz="1200" baseline="0"/>
             <a:t>Description (Optional to title): Description</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0"/>
+            <a:t>url: If your task should not be a screen of text or a command it can open a browser. Type in the url in this field.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0"/>
+            <a:t>it has to start with http:// or https://</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -665,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C11" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -677,7 +709,7 @@
     <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -693,8 +725,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -705,7 +740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -719,43 +754,51 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
@@ -825,7 +868,10 @@
       <c r="B38" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{DA9CD99E-4949-9B4C-9D86-D97191535AB2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>